<commit_message>
corrected data source reset at startTest.
</commit_message>
<xml_diff>
--- a/documentation/Examples/SimpleDataProvider/Simple_Excel_Data.xlsx
+++ b/documentation/Examples/SimpleDataProvider/Simple_Excel_Data.xlsx
@@ -24,18 +24,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>This is a string</t>
-  </si>
-  <si>
-    <t>And this is another string</t>
-  </si>
-  <si>
-    <t>01/01/1970</t>
-  </si>
-  <si>
-    <t>A text line</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>A 11</t>
+  </si>
+  <si>
+    <t>B 11</t>
+  </si>
+  <si>
+    <t>C 11</t>
+  </si>
+  <si>
+    <t>D 11</t>
+  </si>
+  <si>
+    <t>A 12</t>
+  </si>
+  <si>
+    <t>B 12</t>
+  </si>
+  <si>
+    <t>C 12</t>
+  </si>
+  <si>
+    <t>D 12</t>
+  </si>
+  <si>
+    <t>A 13</t>
+  </si>
+  <si>
+    <t>B 13</t>
+  </si>
+  <si>
+    <t>C 13</t>
+  </si>
+  <si>
+    <t>D 13</t>
   </si>
 </sst>
 </file>
@@ -71,10 +95,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,49 +411,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>43233</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1.0449999999999999</v>
-      </c>
-      <c r="B2" s="1">
-        <v>33052</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>-45.24</v>
-      </c>
-      <c r="B3" s="2">
-        <v>36633</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
one more test added.
</commit_message>
<xml_diff>
--- a/documentation/Examples/SimpleDataProvider/Simple_Excel_Data.xlsx
+++ b/documentation/Examples/SimpleDataProvider/Simple_Excel_Data.xlsx
@@ -413,9 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>